<commit_message>
Agregada la logica para el manejo de usuarios
</commit_message>
<xml_diff>
--- a/Requerimientos_Funcionalidades.xlsx
+++ b/Requerimientos_Funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianSegura\source\repos\JulianSegura\DreamSky_RentShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB653D13-ED3C-45A2-85DA-92F27DAE498C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB40157-3552-498F-8759-39BE4B77624A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{36B2DBCD-6DF9-4A78-AAD9-CBD0FEB410AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Proyecto</t>
   </si>
@@ -198,13 +198,19 @@
   </si>
   <si>
     <t>Samsung A9</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +242,13 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Century GothiC "/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -276,10 +289,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,9 +324,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -653,8 +669,8 @@
   <dimension ref="A1:G193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1727,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E047D3F2-6171-4C5E-B883-B441792B81A1}">
-  <dimension ref="C2:H3"/>
+  <dimension ref="C2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1743,7 +1759,7 @@
     <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8">
+    <row r="2" spans="3:10">
       <c r="C2" t="s">
         <v>47</v>
       </c>
@@ -1763,7 +1779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="3:8">
+    <row r="3" spans="3:10">
       <c r="D3">
         <v>12345</v>
       </c>
@@ -1772,6 +1788,64 @@
       </c>
       <c r="F3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>1466</v>
+      </c>
+      <c r="G11" s="12">
+        <f>F11/F13</f>
+        <v>0.40120415982484947</v>
+      </c>
+      <c r="H11">
+        <v>1640</v>
+      </c>
+      <c r="I11" s="12">
+        <f>H11/H13</f>
+        <v>0.44312348014050257</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>2188</v>
+      </c>
+      <c r="G12" s="12">
+        <f>F12/F13</f>
+        <v>0.59879584017515053</v>
+      </c>
+      <c r="H12">
+        <v>2061</v>
+      </c>
+      <c r="I12" s="12">
+        <f>H12/H13</f>
+        <v>0.55687651985949749</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
+      <c r="F13">
+        <f>SUM(F11:F12)</f>
+        <v>3654</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13">
+        <f>SUM(H11:H12)</f>
+        <v>3701</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="I16">
+        <v>340</v>
+      </c>
+      <c r="J16" s="12">
+        <f>I16/H13</f>
+        <v>9.1867062955957854E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada logica de roles y usuarios
</commit_message>
<xml_diff>
--- a/Requerimientos_Funcionalidades.xlsx
+++ b/Requerimientos_Funcionalidades.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianSegura\source\repos\JulianSegura\DreamSky_RentShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB40157-3552-498F-8759-39BE4B77624A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E15F887-49B4-4A6E-BCB9-EFE4FE969263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{36B2DBCD-6DF9-4A78-AAD9-CBD0FEB410AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Validaciones" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="Validaciones" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requerimientos!$A$4:$G$34</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>Proyecto</t>
   </si>
@@ -200,10 +201,76 @@
     <t>Samsung A9</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>Registra Cliente</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Tipo Documento</t>
+  </si>
+  <si>
+    <t>Numero Documento</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Blabla</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>RD480</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Bodeguero</t>
+  </si>
+  <si>
+    <t>Maestro</t>
+  </si>
+  <si>
+    <t>Almacen</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Rentas</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Permisos</t>
+  </si>
+  <si>
+    <t>Creaar Usuario</t>
+  </si>
+  <si>
+    <t>Usario</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -265,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -288,12 +355,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -321,10 +474,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +507,137 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Plus Sign 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50AC4FF3-1DE5-4910-B006-6AFC346299F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4695825" y="2619375"/>
+          <a:ext cx="276225" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathPlus">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Speech Bubble: Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0484F55C-89B8-4AA2-84C2-D0DAC387EB0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="2600325"/>
+          <a:ext cx="257175" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeEllipseCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 85689"/>
+            <a:gd name="adj2" fmla="val 85417"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,8 +961,8 @@
   <dimension ref="A1:G193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="4" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,7 +1021,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -742,7 +1034,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
@@ -753,7 +1045,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
@@ -761,7 +1053,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="30">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
@@ -769,7 +1061,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="45">
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
@@ -780,7 +1072,7 @@
       <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -793,7 +1085,7 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
@@ -804,7 +1096,7 @@
       <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
@@ -815,7 +1107,7 @@
       <c r="A13" s="1">
         <v>7</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
@@ -826,7 +1118,7 @@
       <c r="A14" s="1">
         <v>8</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -839,7 +1131,7 @@
       <c r="A15" s="1">
         <v>9</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="5" t="s">
         <v>31</v>
       </c>
@@ -847,7 +1139,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="30">
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
@@ -858,7 +1150,7 @@
       <c r="A17" s="1">
         <v>10</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -871,7 +1163,7 @@
       <c r="A18" s="1">
         <v>11</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="5" t="s">
         <v>33</v>
       </c>
@@ -882,7 +1174,7 @@
       <c r="A19" s="1">
         <v>12</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -897,7 +1189,7 @@
       <c r="A20" s="1">
         <v>13</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="10" t="s">
         <v>42</v>
       </c>
@@ -908,7 +1200,7 @@
       <c r="A21" s="1">
         <v>15</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
@@ -919,7 +1211,7 @@
       <c r="A22" s="1">
         <v>16</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
@@ -932,7 +1224,7 @@
       <c r="A23" s="1">
         <v>17</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
@@ -943,7 +1235,7 @@
       <c r="A24" s="1">
         <v>18</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="5" t="s">
         <v>46</v>
       </c>
@@ -1713,7 +2005,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:H34" xr:uid="{73B9488D-1BC1-4B35-9B52-8605DA72CAA2}">
-    <sortState ref="A5:G37">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:G37">
       <sortCondition ref="A4:A34"/>
     </sortState>
   </autoFilter>
@@ -1746,7 +2038,7 @@
   <dimension ref="C2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,62 +2083,18 @@
       </c>
     </row>
     <row r="11" spans="3:10">
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11">
-        <v>1466</v>
-      </c>
-      <c r="G11" s="12">
-        <f>F11/F13</f>
-        <v>0.40120415982484947</v>
-      </c>
-      <c r="H11">
-        <v>1640</v>
-      </c>
-      <c r="I11" s="12">
-        <f>H11/H13</f>
-        <v>0.44312348014050257</v>
-      </c>
+      <c r="G11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="3:10">
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12">
-        <v>2188</v>
-      </c>
-      <c r="G12" s="12">
-        <f>F12/F13</f>
-        <v>0.59879584017515053</v>
-      </c>
-      <c r="H12">
-        <v>2061</v>
-      </c>
-      <c r="I12" s="12">
-        <f>H12/H13</f>
-        <v>0.55687651985949749</v>
-      </c>
+      <c r="G12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="3:10">
-      <c r="F13">
-        <f>SUM(F11:F12)</f>
-        <v>3654</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13">
-        <f>SUM(H11:H12)</f>
-        <v>3701</v>
-      </c>
+      <c r="G13" s="11"/>
     </row>
     <row r="16" spans="3:10">
-      <c r="I16">
-        <v>340</v>
-      </c>
-      <c r="J16" s="12">
-        <f>I16/H13</f>
-        <v>9.1867062955957854E-2</v>
-      </c>
+      <c r="J16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1854,6 +2102,218 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E83357-BD1D-4810-BF8A-3E635A10A610}">
+  <dimension ref="B1:L22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="13"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="14"/>
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="14"/>
+      <c r="L4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="L5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1">
+        <v>123456778</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="14"/>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="13"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{5E7798D3-29E2-4130-9C77-90E854F3A000}">
+      <formula1>$L$2:$L$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{90C53B61-1DA1-485C-86B4-9D7E74C7A4A8}">
+      <formula1>$J$2:$J$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15" xr:uid="{3AA77902-E33A-4888-A94A-F6F79BE14E44}">
+      <formula1>$L$2:$L$7</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F4336A-1384-4120-91D3-246C49484C47}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C4"/>

</xml_diff>